<commit_message>
update koppeltabel with selectie kolom
</commit_message>
<xml_diff>
--- a/pbelasting/input/190324_koppeltabel.xlsx
+++ b/pbelasting/input/190324_koppeltabel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1729.N.19 AGV data analyse\WaternetAnalyse\pbelasting\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58999CAB-F88D-4209-BBA9-A2E93A41E1A8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04607584-810B-4709-922C-F4DEFD3FBEC2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3481" uniqueCount="1161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3513" uniqueCount="1163">
   <si>
     <t>2010-GAF_F002.xlsx</t>
   </si>
@@ -3519,6 +3519,12 @@
   </si>
   <si>
     <t>versie2</t>
+  </si>
+  <si>
+    <t>6530-GAF</t>
+  </si>
+  <si>
+    <t>vader</t>
   </si>
 </sst>
 </file>
@@ -5622,7 +5628,7 @@
   <dimension ref="A1:K259"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D228" sqref="D228"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6292,6 +6298,9 @@
       <c r="A26" s="17" t="s">
         <v>1103</v>
       </c>
+      <c r="B26" t="s">
+        <v>560</v>
+      </c>
       <c r="D26">
         <v>0</v>
       </c>
@@ -6623,6 +6632,9 @@
       <c r="A40" t="s">
         <v>621</v>
       </c>
+      <c r="B40" t="s">
+        <v>242</v>
+      </c>
       <c r="D40">
         <v>0</v>
       </c>
@@ -6631,6 +6643,9 @@
       <c r="A41" s="17" t="s">
         <v>1081</v>
       </c>
+      <c r="B41" t="s">
+        <v>242</v>
+      </c>
       <c r="D41">
         <v>0</v>
       </c>
@@ -6668,6 +6683,9 @@
       <c r="A43" t="s">
         <v>33</v>
       </c>
+      <c r="B43" t="s">
+        <v>242</v>
+      </c>
       <c r="C43" t="s">
         <v>243</v>
       </c>
@@ -6679,6 +6697,9 @@
       <c r="A44" t="s">
         <v>622</v>
       </c>
+      <c r="B44" t="s">
+        <v>624</v>
+      </c>
       <c r="D44">
         <v>0</v>
       </c>
@@ -6687,6 +6708,9 @@
       <c r="A45" s="17" t="s">
         <v>1074</v>
       </c>
+      <c r="B45" t="s">
+        <v>624</v>
+      </c>
       <c r="D45">
         <v>0</v>
       </c>
@@ -6724,6 +6748,9 @@
       <c r="A47" t="s">
         <v>619</v>
       </c>
+      <c r="B47" t="s">
+        <v>244</v>
+      </c>
       <c r="D47">
         <v>0</v>
       </c>
@@ -6732,6 +6759,9 @@
       <c r="A48" s="17" t="s">
         <v>1070</v>
       </c>
+      <c r="B48" t="s">
+        <v>244</v>
+      </c>
       <c r="D48">
         <v>1</v>
       </c>
@@ -6769,6 +6799,9 @@
       <c r="A50" t="s">
         <v>34</v>
       </c>
+      <c r="B50" t="s">
+        <v>244</v>
+      </c>
       <c r="C50" t="s">
         <v>214</v>
       </c>
@@ -6789,6 +6822,9 @@
       <c r="A51" t="s">
         <v>620</v>
       </c>
+      <c r="B51" t="s">
+        <v>245</v>
+      </c>
       <c r="D51">
         <v>0</v>
       </c>
@@ -6829,6 +6865,9 @@
       <c r="A53" s="17" t="s">
         <v>1063</v>
       </c>
+      <c r="B53" t="s">
+        <v>245</v>
+      </c>
       <c r="D53">
         <v>0</v>
       </c>
@@ -6837,6 +6876,9 @@
       <c r="A54" t="s">
         <v>35</v>
       </c>
+      <c r="B54" t="s">
+        <v>245</v>
+      </c>
       <c r="D54">
         <v>0</v>
       </c>
@@ -6845,6 +6887,9 @@
       <c r="A55" t="s">
         <v>618</v>
       </c>
+      <c r="B55" t="s">
+        <v>623</v>
+      </c>
       <c r="D55">
         <v>1</v>
       </c>
@@ -6871,6 +6916,9 @@
       <c r="A56" s="17" t="s">
         <v>1058</v>
       </c>
+      <c r="B56" t="s">
+        <v>246</v>
+      </c>
       <c r="D56">
         <v>1</v>
       </c>
@@ -6879,6 +6927,9 @@
       <c r="A57" t="s">
         <v>36</v>
       </c>
+      <c r="B57" t="s">
+        <v>246</v>
+      </c>
       <c r="D57">
         <v>0</v>
       </c>
@@ -6942,6 +6993,9 @@
       <c r="A60" t="s">
         <v>37</v>
       </c>
+      <c r="B60" t="s">
+        <v>248</v>
+      </c>
       <c r="D60">
         <v>1</v>
       </c>
@@ -6959,6 +7013,9 @@
       <c r="A61" t="s">
         <v>38</v>
       </c>
+      <c r="B61" t="s">
+        <v>248</v>
+      </c>
       <c r="D61">
         <v>2</v>
       </c>
@@ -7002,6 +7059,9 @@
       <c r="A63" s="17" t="s">
         <v>1044</v>
       </c>
+      <c r="B63" t="s">
+        <v>248</v>
+      </c>
       <c r="D63">
         <v>0</v>
       </c>
@@ -7236,6 +7296,9 @@
       <c r="A72" t="s">
         <v>45</v>
       </c>
+      <c r="B72" t="s">
+        <v>254</v>
+      </c>
       <c r="D72">
         <v>3</v>
       </c>
@@ -7302,8 +7365,8 @@
       <c r="A75" t="s">
         <v>50</v>
       </c>
-      <c r="B75">
-        <v>2501</v>
+      <c r="B75" t="s">
+        <v>256</v>
       </c>
       <c r="C75" t="s">
         <v>258</v>
@@ -7331,8 +7394,8 @@
       <c r="A76" t="s">
         <v>49</v>
       </c>
-      <c r="B76">
-        <v>2501</v>
+      <c r="B76" t="s">
+        <v>256</v>
       </c>
       <c r="C76" t="s">
         <v>258</v>
@@ -7733,6 +7796,9 @@
       <c r="A91" t="s">
         <v>614</v>
       </c>
+      <c r="B91" t="s">
+        <v>271</v>
+      </c>
       <c r="D91">
         <v>0</v>
       </c>
@@ -8369,6 +8435,9 @@
       <c r="A117" s="12" t="s">
         <v>616</v>
       </c>
+      <c r="B117" t="s">
+        <v>284</v>
+      </c>
       <c r="C117" t="s">
         <v>247</v>
       </c>
@@ -8763,8 +8832,8 @@
       <c r="A133" t="s">
         <v>99</v>
       </c>
-      <c r="B133">
-        <v>3220</v>
+      <c r="B133" t="s">
+        <v>393</v>
       </c>
       <c r="C133" t="s">
         <v>296</v>
@@ -8815,8 +8884,8 @@
       <c r="A135" t="s">
         <v>110</v>
       </c>
-      <c r="B135">
-        <v>3230</v>
+      <c r="B135" t="s">
+        <v>303</v>
       </c>
       <c r="C135" t="s">
         <v>305</v>
@@ -9787,6 +9856,9 @@
       <c r="A172" t="s">
         <v>540</v>
       </c>
+      <c r="B172" t="s">
+        <v>323</v>
+      </c>
       <c r="C172" t="s">
         <v>539</v>
       </c>
@@ -9816,6 +9888,9 @@
       <c r="A173" t="s">
         <v>615</v>
       </c>
+      <c r="B173" t="s">
+        <v>323</v>
+      </c>
       <c r="D173">
         <v>0</v>
       </c>
@@ -10406,8 +10481,8 @@
       <c r="A195" t="s">
         <v>156</v>
       </c>
-      <c r="B195">
-        <v>4000</v>
+      <c r="B195" t="s">
+        <v>342</v>
       </c>
       <c r="C195" t="s">
         <v>345</v>
@@ -11370,8 +11445,8 @@
       <c r="A234" t="s">
         <v>189</v>
       </c>
-      <c r="B234">
-        <v>6530</v>
+      <c r="B234" t="s">
+        <v>1161</v>
       </c>
       <c r="C234" t="s">
         <v>214</v>
@@ -11393,8 +11468,8 @@
       <c r="A235" t="s">
         <v>190</v>
       </c>
-      <c r="B235">
-        <v>6530</v>
+      <c r="B235" t="s">
+        <v>1161</v>
       </c>
       <c r="C235" t="s">
         <v>212</v>
@@ -11416,8 +11491,8 @@
       <c r="A236" t="s">
         <v>191</v>
       </c>
-      <c r="B236">
-        <v>6530</v>
+      <c r="B236" t="s">
+        <v>1161</v>
       </c>
       <c r="C236" t="s">
         <v>217</v>
@@ -11968,6 +12043,9 @@
     <row r="259" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A259" s="13" t="s">
         <v>593</v>
+      </c>
+      <c r="B259" t="s">
+        <v>1162</v>
       </c>
       <c r="D259">
         <v>0</v>
@@ -24070,6 +24148,88 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Classificatie xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">Intern</Classificatie>
+    <Entiteit_x0020_type xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">Record</Entiteit_x0020_type>
+    <_dlc_DocId xmlns="fbe582d4-4cd9-4e01-adc0-428c7d30a990">PNHZET2ZRHHM-1647798991-93060</_dlc_DocId>
+    <Aggregatieniveau xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">Archiefstuk</Aggregatieniveau>
+    <TaxCatchAll xmlns="d59e9867-4acc-40d5-91da-91f4047d1695"/>
+    <Omschrijving xmlns="d59e9867-4acc-40d5-91da-91f4047d1695" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Aanmaakdatum xmlns="d59e9867-4acc-40d5-91da-91f4047d1695" xsi:nil="true"/>
+    <Document_x0020_type xmlns="d59e9867-4acc-40d5-91da-91f4047d1695" xsi:nil="true"/>
+    <_dlc_DocIdUrl xmlns="fbe582d4-4cd9-4e01-adc0-428c7d30a990">
+      <Url>https://waternet.sharepoint.com/sites/0182/_layouts/15/DocIdRedir.aspx?ID=PNHZET2ZRHHM-1647798991-93060</Url>
+      <Description>PNHZET2ZRHHM-1647798991-93060</Description>
+    </_dlc_DocIdUrl>
+    <Identificatiekenmerk xmlns="d59e9867-4acc-40d5-91da-91f4047d1695" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Algemeen - Word" ma:contentTypeID="0x0101004F34529632943E4DBB820B36F0ABAA0606010086381A6D56669A4DB59F7772448721B1" ma:contentTypeVersion="5" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="8fe95572a7a7878b61abe4cdcaa95a61">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d59e9867-4acc-40d5-91da-91f4047d1695" xmlns:ns3="fbe582d4-4cd9-4e01-adc0-428c7d30a990" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b624776c1a3c75443e1a1b758f5efa1" ns2:_="" ns3:_="">
     <xsd:import namespace="d59e9867-4acc-40d5-91da-91f4047d1695"/>
@@ -24369,94 +24529,45 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Classificatie xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">Intern</Classificatie>
-    <Entiteit_x0020_type xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">Record</Entiteit_x0020_type>
-    <_dlc_DocId xmlns="fbe582d4-4cd9-4e01-adc0-428c7d30a990">PNHZET2ZRHHM-1647798991-93060</_dlc_DocId>
-    <Aggregatieniveau xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">Archiefstuk</Aggregatieniveau>
-    <TaxCatchAll xmlns="d59e9867-4acc-40d5-91da-91f4047d1695"/>
-    <Omschrijving xmlns="d59e9867-4acc-40d5-91da-91f4047d1695" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <Aanmaakdatum xmlns="d59e9867-4acc-40d5-91da-91f4047d1695" xsi:nil="true"/>
-    <Document_x0020_type xmlns="d59e9867-4acc-40d5-91da-91f4047d1695" xsi:nil="true"/>
-    <_dlc_DocIdUrl xmlns="fbe582d4-4cd9-4e01-adc0-428c7d30a990">
-      <Url>https://waternet.sharepoint.com/sites/0182/_layouts/15/DocIdRedir.aspx?ID=PNHZET2ZRHHM-1647798991-93060</Url>
-      <Description>PNHZET2ZRHHM-1647798991-93060</Description>
-    </_dlc_DocIdUrl>
-    <Identificatiekenmerk xmlns="d59e9867-4acc-40d5-91da-91f4047d1695" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="7c1d69d6-3248-424b-85a1-c0d9ad05b603" ContentTypeId="0x0101004F34529632943E4DBB820B36F0ABAA060601" PreviousValue="false"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C93CFFD-81C7-408F-9360-B07E2D660303}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D2BE5C7-D2B0-4B18-9D85-BE52E70FE1F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{629D2343-3DBC-4425-9979-C53AF3E8F60A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="fbe582d4-4cd9-4e01-adc0-428c7d30a990"/>
+    <ds:schemaRef ds:uri="d59e9867-4acc-40d5-91da-91f4047d1695"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{743CA991-A91A-4ABA-A663-E5C279512219}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24475,39 +24586,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{629D2343-3DBC-4425-9979-C53AF3E8F60A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="fbe582d4-4cd9-4e01-adc0-428c7d30a990"/>
-    <ds:schemaRef ds:uri="d59e9867-4acc-40d5-91da-91f4047d1695"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D2BE5C7-D2B0-4B18-9D85-BE52E70FE1F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C93CFFD-81C7-408F-9360-B07E2D660303}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A66FD23B-6941-41A1-8A1A-FC46E735FC7F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
add change koppeltabel wabalans
</commit_message>
<xml_diff>
--- a/pbelasting/input/190324_koppeltabel.xlsx
+++ b/pbelasting/input/190324_koppeltabel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1729.N.19 AGV data analyse\WaternetAnalyse\pbelasting\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04607584-810B-4709-922C-F4DEFD3FBEC2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC316AE-E1C1-4945-96BA-49231FA63014}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
@@ -3710,7 +3710,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3905,6 +3905,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF4E5C68"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4105,7 +4111,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4143,6 +4149,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5627,15 +5634,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K259"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A247" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E256" sqref="E256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="60.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="19"/>
+    <col min="6" max="6" width="12" style="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.7109375" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" customWidth="1"/>
     <col min="11" max="11" width="9.140625" style="5"/>
@@ -5654,10 +5662,10 @@
       <c r="D1" t="s">
         <v>1160</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="19" t="s">
         <v>389</v>
       </c>
       <c r="G1" t="s">
@@ -5689,7 +5697,7 @@
       <c r="D2">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="19">
         <v>2010</v>
       </c>
       <c r="G2" t="s">
@@ -5738,7 +5746,7 @@
       <c r="D4">
         <v>2</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="19">
         <v>2100</v>
       </c>
       <c r="G4" t="s">
@@ -5764,7 +5772,7 @@
       <c r="D5">
         <v>2</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="19">
         <v>2110</v>
       </c>
       <c r="G5" t="s">
@@ -5842,7 +5850,7 @@
       <c r="D8">
         <v>4</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="19">
         <v>2120</v>
       </c>
       <c r="G8" t="s">
@@ -5874,7 +5882,7 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="19" t="s">
         <v>219</v>
       </c>
       <c r="G9" t="s">
@@ -5923,7 +5931,7 @@
       <c r="D11">
         <v>0</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="19">
         <v>2130</v>
       </c>
       <c r="G11" t="s">
@@ -5955,7 +5963,7 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="19" t="s">
         <v>223</v>
       </c>
       <c r="G12" t="s">
@@ -5981,7 +5989,7 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="19" t="s">
         <v>224</v>
       </c>
       <c r="G13" t="s">
@@ -6030,7 +6038,7 @@
       <c r="D15">
         <v>2</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="19">
         <v>2140</v>
       </c>
       <c r="G15" t="s">
@@ -6056,7 +6064,7 @@
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="19">
         <v>2150</v>
       </c>
       <c r="G16" t="s">
@@ -6105,7 +6113,7 @@
       <c r="D18">
         <v>3</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="19">
         <v>2210</v>
       </c>
       <c r="G18" t="s">
@@ -6165,7 +6173,7 @@
       <c r="D21">
         <v>2</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="19" t="s">
         <v>587</v>
       </c>
       <c r="G21" t="s">
@@ -6197,7 +6205,7 @@
       <c r="D22">
         <v>2</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="19">
         <v>2220</v>
       </c>
       <c r="G22" t="s">
@@ -6223,7 +6231,7 @@
       <c r="D23">
         <v>2</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="19">
         <v>2230</v>
       </c>
       <c r="G23" t="s">
@@ -6249,7 +6257,7 @@
       <c r="D24">
         <v>2</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="19">
         <v>2240</v>
       </c>
       <c r="G24" t="s">
@@ -6275,7 +6283,7 @@
       <c r="D25">
         <v>2</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="19" t="s">
         <v>560</v>
       </c>
       <c r="G25" t="s">
@@ -6318,7 +6326,7 @@
       <c r="D27">
         <v>2</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="19" t="s">
         <v>231</v>
       </c>
       <c r="G27" t="s">
@@ -6344,7 +6352,7 @@
       <c r="D28">
         <v>3</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="19">
         <v>2250</v>
       </c>
       <c r="G28" t="s">
@@ -6370,7 +6378,7 @@
       <c r="D29">
         <v>2</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="19">
         <v>2270</v>
       </c>
       <c r="G29" t="s">
@@ -6442,7 +6450,7 @@
       <c r="D32">
         <v>2</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="19">
         <v>2290</v>
       </c>
       <c r="G32" t="s">
@@ -6468,7 +6476,7 @@
       <c r="D33">
         <v>2</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="19">
         <v>2300</v>
       </c>
       <c r="G33" t="s">
@@ -6494,7 +6502,7 @@
       <c r="D34">
         <v>2</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="19">
         <v>2310</v>
       </c>
       <c r="G34" t="s">
@@ -6566,7 +6574,7 @@
       <c r="D37">
         <v>3</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="19">
         <v>2330</v>
       </c>
       <c r="G37" t="s">
@@ -6592,7 +6600,7 @@
       <c r="D38">
         <v>2</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="19">
         <v>2340</v>
       </c>
       <c r="G38" t="s">
@@ -6660,7 +6668,7 @@
       <c r="D42">
         <v>3</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="19" t="s">
         <v>242</v>
       </c>
       <c r="G42" t="s">
@@ -6725,7 +6733,7 @@
       <c r="D46">
         <v>3</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="19" t="s">
         <v>624</v>
       </c>
       <c r="G46" t="s">
@@ -6776,7 +6784,7 @@
       <c r="D49">
         <v>0</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="19" t="s">
         <v>244</v>
       </c>
       <c r="G49" t="s">
@@ -6842,7 +6850,7 @@
       <c r="D52">
         <v>1</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="19" t="s">
         <v>245</v>
       </c>
       <c r="G52" t="s">
@@ -6893,7 +6901,7 @@
       <c r="D55">
         <v>1</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="19" t="s">
         <v>623</v>
       </c>
       <c r="G55" t="s">
@@ -6953,7 +6961,7 @@
       <c r="D58">
         <v>4</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="19" t="s">
         <v>246</v>
       </c>
       <c r="G58" t="s">
@@ -7042,7 +7050,7 @@
       <c r="D62">
         <v>3</v>
       </c>
-      <c r="E62">
+      <c r="E62" s="19">
         <v>2400</v>
       </c>
       <c r="G62" t="s">
@@ -7079,7 +7087,7 @@
       <c r="D64">
         <v>2</v>
       </c>
-      <c r="E64">
+      <c r="E64" s="19">
         <v>2410</v>
       </c>
       <c r="G64" t="s">
@@ -7105,7 +7113,7 @@
       <c r="D65">
         <v>1</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="19" t="s">
         <v>250</v>
       </c>
       <c r="G65" t="s">
@@ -7134,7 +7142,7 @@
       <c r="D66">
         <v>1</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" s="19" t="s">
         <v>584</v>
       </c>
       <c r="G66" t="s">
@@ -7166,7 +7174,7 @@
       <c r="D67">
         <v>1</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="19" t="s">
         <v>585</v>
       </c>
       <c r="G67" t="s">
@@ -7198,7 +7206,7 @@
       <c r="D68">
         <v>1</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68" s="19" t="s">
         <v>253</v>
       </c>
       <c r="G68" t="s">
@@ -7253,7 +7261,7 @@
       <c r="D70">
         <v>1</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F70" s="19" t="s">
         <v>254</v>
       </c>
       <c r="G70" t="s">
@@ -7279,7 +7287,7 @@
       <c r="D71">
         <v>2</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F71" s="19" t="s">
         <v>254</v>
       </c>
       <c r="G71" t="s">
@@ -7316,7 +7324,7 @@
       <c r="D73">
         <v>4</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F73" s="19" t="s">
         <v>254</v>
       </c>
       <c r="G73" t="s">
@@ -7348,7 +7356,7 @@
       <c r="D74">
         <v>1</v>
       </c>
-      <c r="E74">
+      <c r="E74" s="19">
         <v>2500</v>
       </c>
       <c r="G74" t="s">
@@ -7374,7 +7382,7 @@
       <c r="D75">
         <v>0</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F75" s="19" t="s">
         <v>256</v>
       </c>
       <c r="G75" t="s">
@@ -7403,7 +7411,7 @@
       <c r="D76">
         <v>0</v>
       </c>
-      <c r="E76">
+      <c r="E76" s="19">
         <v>2501</v>
       </c>
       <c r="G76" t="s">
@@ -7432,7 +7440,7 @@
       <c r="D77">
         <v>1</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F77" s="19" t="s">
         <v>256</v>
       </c>
       <c r="G77" t="s">
@@ -7458,7 +7466,7 @@
       <c r="D78">
         <v>1</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F78" s="19" t="s">
         <v>257</v>
       </c>
       <c r="G78" t="s">
@@ -7484,7 +7492,7 @@
       <c r="D79">
         <v>1</v>
       </c>
-      <c r="E79">
+      <c r="E79" s="19">
         <v>2502</v>
       </c>
       <c r="G79" t="s">
@@ -7510,7 +7518,7 @@
       <c r="D80">
         <v>1</v>
       </c>
-      <c r="E80">
+      <c r="E80" s="19">
         <v>2503</v>
       </c>
       <c r="G80" t="s">
@@ -7536,7 +7544,7 @@
       <c r="D81">
         <v>2</v>
       </c>
-      <c r="E81">
+      <c r="E81" s="19">
         <v>2504</v>
       </c>
       <c r="G81" t="s">
@@ -7562,7 +7570,7 @@
       <c r="D82">
         <v>1</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F82" s="19" t="s">
         <v>262</v>
       </c>
       <c r="G82" t="s">
@@ -7588,7 +7596,7 @@
       <c r="D83">
         <v>1</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F83" s="19" t="s">
         <v>547</v>
       </c>
       <c r="G83" t="s">
@@ -7614,7 +7622,7 @@
       <c r="D84">
         <v>1</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F84" s="19" t="s">
         <v>264</v>
       </c>
       <c r="G84" t="s">
@@ -7640,7 +7648,7 @@
       <c r="D85">
         <v>1</v>
       </c>
-      <c r="F85" t="s">
+      <c r="F85" s="19" t="s">
         <v>265</v>
       </c>
       <c r="G85" t="s">
@@ -7666,7 +7674,7 @@
       <c r="D86">
         <v>1</v>
       </c>
-      <c r="E86">
+      <c r="E86" s="19">
         <v>2510</v>
       </c>
       <c r="G86" t="s">
@@ -7695,7 +7703,7 @@
       <c r="D87">
         <v>1</v>
       </c>
-      <c r="E87">
+      <c r="E87" s="19">
         <v>2511</v>
       </c>
       <c r="G87" t="s">
@@ -7721,7 +7729,7 @@
       <c r="D88">
         <v>2</v>
       </c>
-      <c r="E88">
+      <c r="E88" s="19">
         <v>2520</v>
       </c>
       <c r="G88" t="s">
@@ -7747,7 +7755,7 @@
       <c r="D89">
         <v>2</v>
       </c>
-      <c r="E89">
+      <c r="E89" s="19">
         <v>2530</v>
       </c>
       <c r="G89" t="s">
@@ -7773,7 +7781,7 @@
       <c r="D90">
         <v>2</v>
       </c>
-      <c r="E90">
+      <c r="E90" s="19">
         <v>2540</v>
       </c>
       <c r="G90" t="s">
@@ -7802,7 +7810,7 @@
       <c r="D91">
         <v>0</v>
       </c>
-      <c r="E91">
+      <c r="E91" s="19">
         <v>2400</v>
       </c>
       <c r="K91"/>
@@ -7843,7 +7851,7 @@
       <c r="D93">
         <v>3</v>
       </c>
-      <c r="E93">
+      <c r="E93" s="19">
         <v>2550</v>
       </c>
       <c r="G93" t="s">
@@ -7875,7 +7883,7 @@
       <c r="D94">
         <v>2</v>
       </c>
-      <c r="E94">
+      <c r="E94" s="19">
         <v>2560</v>
       </c>
       <c r="G94" t="s">
@@ -7924,7 +7932,7 @@
       <c r="D96">
         <v>3</v>
       </c>
-      <c r="E96">
+      <c r="E96" s="19">
         <v>2570</v>
       </c>
       <c r="G96" t="s">
@@ -7973,7 +7981,7 @@
       <c r="D98">
         <v>3</v>
       </c>
-      <c r="E98">
+      <c r="E98" s="19">
         <v>2600</v>
       </c>
       <c r="G98" t="s">
@@ -8028,7 +8036,7 @@
       <c r="D100">
         <v>3</v>
       </c>
-      <c r="E100">
+      <c r="E100" s="19">
         <v>2610</v>
       </c>
       <c r="G100" t="s">
@@ -8100,7 +8108,7 @@
       <c r="D103">
         <v>3</v>
       </c>
-      <c r="E103">
+      <c r="E103" s="19">
         <v>2620</v>
       </c>
       <c r="G103" t="s">
@@ -8126,7 +8134,7 @@
       <c r="D104">
         <v>2</v>
       </c>
-      <c r="F104" t="s">
+      <c r="F104" s="19" t="s">
         <v>608</v>
       </c>
       <c r="G104" t="s">
@@ -8170,7 +8178,7 @@
       <c r="D106">
         <v>2</v>
       </c>
-      <c r="E106">
+      <c r="E106" s="19">
         <v>2630</v>
       </c>
       <c r="G106" t="s">
@@ -8196,7 +8204,7 @@
       <c r="D107">
         <v>2</v>
       </c>
-      <c r="F107" t="s">
+      <c r="F107" s="19" t="s">
         <v>548</v>
       </c>
       <c r="G107" t="s">
@@ -8245,7 +8253,7 @@
       <c r="D109">
         <v>3</v>
       </c>
-      <c r="E109">
+      <c r="E109" s="19">
         <v>3020</v>
       </c>
       <c r="G109" t="s">
@@ -8294,7 +8302,7 @@
       <c r="D111">
         <v>2</v>
       </c>
-      <c r="F111" t="s">
+      <c r="F111" s="19" t="s">
         <v>281</v>
       </c>
       <c r="G111" t="s">
@@ -8343,7 +8351,7 @@
       <c r="D113">
         <v>2</v>
       </c>
-      <c r="F113" t="s">
+      <c r="F113" s="19" t="s">
         <v>282</v>
       </c>
       <c r="G113" t="s">
@@ -8392,7 +8400,7 @@
       <c r="D115">
         <v>3</v>
       </c>
-      <c r="E115">
+      <c r="E115" s="19">
         <v>3070</v>
       </c>
       <c r="G115" t="s">
@@ -8444,7 +8452,7 @@
       <c r="D117">
         <v>0</v>
       </c>
-      <c r="E117">
+      <c r="E117" s="19">
         <v>3100</v>
       </c>
       <c r="G117" t="s">
@@ -8476,7 +8484,7 @@
       <c r="D118">
         <v>1</v>
       </c>
-      <c r="F118" t="s">
+      <c r="F118" s="19" t="s">
         <v>285</v>
       </c>
       <c r="G118" t="s">
@@ -8502,7 +8510,7 @@
       <c r="D119">
         <v>2</v>
       </c>
-      <c r="F119" t="s">
+      <c r="F119" s="19" t="s">
         <v>550</v>
       </c>
       <c r="G119" t="s">
@@ -8528,7 +8536,7 @@
       <c r="D120">
         <v>1</v>
       </c>
-      <c r="F120" t="s">
+      <c r="F120" s="19" t="s">
         <v>287</v>
       </c>
       <c r="G120" t="s">
@@ -8577,7 +8585,7 @@
       <c r="D122">
         <v>0</v>
       </c>
-      <c r="E122">
+      <c r="E122" s="19">
         <v>3200</v>
       </c>
       <c r="G122" t="s">
@@ -8632,7 +8640,7 @@
       <c r="D124">
         <v>2</v>
       </c>
-      <c r="F124" t="s">
+      <c r="F124" s="19" t="s">
         <v>289</v>
       </c>
       <c r="G124" t="s">
@@ -8710,7 +8718,7 @@
       <c r="D127">
         <v>2</v>
       </c>
-      <c r="F127" t="s">
+      <c r="F127" s="19" t="s">
         <v>292</v>
       </c>
       <c r="G127" t="s">
@@ -8759,7 +8767,7 @@
       <c r="D129">
         <v>2</v>
       </c>
-      <c r="F129" t="s">
+      <c r="F129" s="19" t="s">
         <v>293</v>
       </c>
       <c r="G129" t="s">
@@ -8785,7 +8793,7 @@
       <c r="D130">
         <v>1</v>
       </c>
-      <c r="E130">
+      <c r="E130" s="19">
         <v>3210</v>
       </c>
       <c r="G130" t="s">
@@ -8841,7 +8849,7 @@
       <c r="D133">
         <v>1</v>
       </c>
-      <c r="F133" t="s">
+      <c r="F133" s="19" t="s">
         <v>393</v>
       </c>
       <c r="G133" t="s">
@@ -8867,7 +8875,7 @@
       <c r="D134">
         <v>1</v>
       </c>
-      <c r="E134">
+      <c r="E134" s="19">
         <v>3220</v>
       </c>
       <c r="G134" t="s">
@@ -8893,7 +8901,7 @@
       <c r="D135">
         <v>1</v>
       </c>
-      <c r="F135" t="s">
+      <c r="F135" s="19" t="s">
         <v>303</v>
       </c>
       <c r="G135" t="s">
@@ -8948,7 +8956,7 @@
       <c r="D137">
         <v>2</v>
       </c>
-      <c r="F137" t="s">
+      <c r="F137" s="19" t="s">
         <v>297</v>
       </c>
       <c r="G137" t="s">
@@ -9003,7 +9011,7 @@
       <c r="D139">
         <v>2</v>
       </c>
-      <c r="F139" t="s">
+      <c r="F139" s="19" t="s">
         <v>298</v>
       </c>
       <c r="G139" t="s">
@@ -9058,7 +9066,7 @@
       <c r="D141">
         <v>2</v>
       </c>
-      <c r="F141" t="s">
+      <c r="F141" s="19" t="s">
         <v>299</v>
       </c>
       <c r="G141" t="s">
@@ -9090,7 +9098,7 @@
       <c r="D142">
         <v>1</v>
       </c>
-      <c r="F142" t="s">
+      <c r="F142" s="19" t="s">
         <v>302</v>
       </c>
       <c r="G142" t="s">
@@ -9139,7 +9147,7 @@
       <c r="D144">
         <v>1</v>
       </c>
-      <c r="F144" t="s">
+      <c r="F144" s="19" t="s">
         <v>303</v>
       </c>
       <c r="G144" t="s">
@@ -9165,7 +9173,7 @@
       <c r="D145">
         <v>1</v>
       </c>
-      <c r="E145">
+      <c r="E145" s="19">
         <v>3230</v>
       </c>
       <c r="G145" t="s">
@@ -9191,7 +9199,7 @@
       <c r="D146">
         <v>2</v>
       </c>
-      <c r="E146">
+      <c r="E146" s="19">
         <v>3240</v>
       </c>
       <c r="G146" t="s">
@@ -9217,7 +9225,7 @@
       <c r="D147">
         <v>2</v>
       </c>
-      <c r="F147" t="s">
+      <c r="F147" s="19" t="s">
         <v>307</v>
       </c>
       <c r="G147" t="s">
@@ -9243,7 +9251,7 @@
       <c r="D148">
         <v>0</v>
       </c>
-      <c r="F148" t="s">
+      <c r="F148" s="19" t="s">
         <v>551</v>
       </c>
       <c r="G148" t="s">
@@ -9269,7 +9277,7 @@
       <c r="D149">
         <v>1</v>
       </c>
-      <c r="F149" t="s">
+      <c r="F149" s="19" t="s">
         <v>588</v>
       </c>
       <c r="G149" t="s">
@@ -9295,7 +9303,7 @@
       <c r="D150">
         <v>0</v>
       </c>
-      <c r="F150" t="s">
+      <c r="F150" s="19" t="s">
         <v>552</v>
       </c>
       <c r="G150" t="s">
@@ -9321,7 +9329,7 @@
       <c r="D151">
         <v>1</v>
       </c>
-      <c r="F151" t="s">
+      <c r="F151" s="19" t="s">
         <v>589</v>
       </c>
       <c r="G151" t="s">
@@ -9347,7 +9355,7 @@
       <c r="D152">
         <v>1</v>
       </c>
-      <c r="F152" t="s">
+      <c r="F152" s="19" t="s">
         <v>553</v>
       </c>
       <c r="G152" t="s">
@@ -9370,7 +9378,7 @@
       <c r="D153">
         <v>1</v>
       </c>
-      <c r="F153" t="s">
+      <c r="F153" s="19" t="s">
         <v>590</v>
       </c>
       <c r="G153" t="s">
@@ -9399,7 +9407,7 @@
       <c r="D154">
         <v>0</v>
       </c>
-      <c r="F154" t="s">
+      <c r="F154" s="19" t="s">
         <v>551</v>
       </c>
       <c r="G154" t="s">
@@ -9428,7 +9436,7 @@
       <c r="D155">
         <v>0</v>
       </c>
-      <c r="F155" t="s">
+      <c r="F155" s="19" t="s">
         <v>591</v>
       </c>
       <c r="G155" t="s">
@@ -9457,7 +9465,7 @@
       <c r="D156">
         <v>0</v>
       </c>
-      <c r="F156" t="s">
+      <c r="F156" s="19" t="s">
         <v>592</v>
       </c>
       <c r="G156" t="s">
@@ -9510,7 +9518,7 @@
         <v>247</v>
       </c>
       <c r="D158">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K158"/>
     </row>
@@ -9525,9 +9533,9 @@
         <v>247</v>
       </c>
       <c r="D159">
-        <v>0</v>
-      </c>
-      <c r="E159">
+        <v>2</v>
+      </c>
+      <c r="E159" s="19">
         <v>3300</v>
       </c>
       <c r="G159" t="s">
@@ -9556,7 +9564,7 @@
       <c r="D160">
         <v>2</v>
       </c>
-      <c r="F160" t="s">
+      <c r="F160" s="19" t="s">
         <v>312</v>
       </c>
       <c r="G160" t="s">
@@ -9582,7 +9590,7 @@
       <c r="D161">
         <v>2</v>
       </c>
-      <c r="F161" t="s">
+      <c r="F161" s="19" t="s">
         <v>313</v>
       </c>
       <c r="G161" t="s">
@@ -9654,7 +9662,7 @@
       <c r="D164">
         <v>2</v>
       </c>
-      <c r="E164">
+      <c r="E164" s="19">
         <v>3302</v>
       </c>
       <c r="G164" t="s">
@@ -9680,7 +9688,7 @@
       <c r="D165">
         <v>2</v>
       </c>
-      <c r="F165" t="s">
+      <c r="F165" s="19" t="s">
         <v>317</v>
       </c>
       <c r="G165" t="s">
@@ -9706,7 +9714,7 @@
       <c r="D166">
         <v>2</v>
       </c>
-      <c r="E166">
+      <c r="E166" s="19">
         <v>3311</v>
       </c>
       <c r="G166" t="s">
@@ -9732,7 +9740,7 @@
       <c r="D167">
         <v>2</v>
       </c>
-      <c r="F167" t="s">
+      <c r="F167" s="19" t="s">
         <v>555</v>
       </c>
       <c r="G167" t="s">
@@ -9758,7 +9766,7 @@
       <c r="D168">
         <v>2</v>
       </c>
-      <c r="E168">
+      <c r="E168" s="19">
         <v>3350</v>
       </c>
       <c r="G168" t="s">
@@ -9784,7 +9792,7 @@
       <c r="D169">
         <v>2</v>
       </c>
-      <c r="F169" t="s">
+      <c r="F169" s="19" t="s">
         <v>321</v>
       </c>
       <c r="G169" t="s">
@@ -9810,7 +9818,7 @@
       <c r="D170">
         <v>2</v>
       </c>
-      <c r="F170" t="s">
+      <c r="F170" s="19" t="s">
         <v>322</v>
       </c>
       <c r="G170" t="s">
@@ -9865,7 +9873,7 @@
       <c r="D172">
         <v>0</v>
       </c>
-      <c r="F172" t="s">
+      <c r="F172" s="19" t="s">
         <v>323</v>
       </c>
       <c r="G172" t="s">
@@ -9894,7 +9902,7 @@
       <c r="D173">
         <v>0</v>
       </c>
-      <c r="F173" t="s">
+      <c r="F173" s="19" t="s">
         <v>323</v>
       </c>
       <c r="G173" t="s">
@@ -9923,7 +9931,7 @@
       <c r="D174">
         <v>1</v>
       </c>
-      <c r="F174" t="s">
+      <c r="F174" s="19" t="s">
         <v>324</v>
       </c>
       <c r="G174" t="s">
@@ -9955,7 +9963,7 @@
       <c r="D175">
         <v>1</v>
       </c>
-      <c r="F175" t="s">
+      <c r="F175" s="19" t="s">
         <v>325</v>
       </c>
       <c r="G175" t="s">
@@ -9987,7 +9995,7 @@
       <c r="D176">
         <v>2</v>
       </c>
-      <c r="F176" t="s">
+      <c r="F176" s="19" t="s">
         <v>326</v>
       </c>
       <c r="G176" t="s">
@@ -10019,7 +10027,7 @@
       <c r="D177">
         <v>2</v>
       </c>
-      <c r="F177" t="s">
+      <c r="F177" s="19" t="s">
         <v>327</v>
       </c>
       <c r="G177" t="s">
@@ -10068,7 +10076,7 @@
       <c r="D179">
         <v>0</v>
       </c>
-      <c r="F179" t="s">
+      <c r="F179" s="19" t="s">
         <v>328</v>
       </c>
       <c r="G179" t="s">
@@ -10123,7 +10131,7 @@
       <c r="D181">
         <v>0</v>
       </c>
-      <c r="F181" t="s">
+      <c r="F181" s="19" t="s">
         <v>329</v>
       </c>
       <c r="G181" t="s">
@@ -10155,7 +10163,7 @@
       <c r="D182">
         <v>2</v>
       </c>
-      <c r="F182" t="s">
+      <c r="F182" s="19" t="s">
         <v>330</v>
       </c>
       <c r="G182" t="s">
@@ -10204,7 +10212,7 @@
       <c r="D184">
         <v>3</v>
       </c>
-      <c r="F184" t="s">
+      <c r="F184" s="19" t="s">
         <v>331</v>
       </c>
       <c r="G184" t="s">
@@ -10230,7 +10238,7 @@
       <c r="D185">
         <v>2</v>
       </c>
-      <c r="F185" t="s">
+      <c r="F185" s="19" t="s">
         <v>332</v>
       </c>
       <c r="G185" t="s">
@@ -10256,7 +10264,7 @@
       <c r="D186">
         <v>2</v>
       </c>
-      <c r="F186" t="s">
+      <c r="F186" s="19" t="s">
         <v>333</v>
       </c>
       <c r="G186" t="s">
@@ -10282,7 +10290,7 @@
       <c r="D187">
         <v>2</v>
       </c>
-      <c r="F187" t="s">
+      <c r="F187" s="19" t="s">
         <v>334</v>
       </c>
       <c r="G187" t="s">
@@ -10308,7 +10316,7 @@
       <c r="D188">
         <v>2</v>
       </c>
-      <c r="F188" t="s">
+      <c r="F188" s="19" t="s">
         <v>335</v>
       </c>
       <c r="G188" t="s">
@@ -10334,7 +10342,7 @@
       <c r="D189">
         <v>2</v>
       </c>
-      <c r="F189" t="s">
+      <c r="F189" s="19" t="s">
         <v>336</v>
       </c>
       <c r="G189" t="s">
@@ -10360,7 +10368,7 @@
       <c r="D190">
         <v>2</v>
       </c>
-      <c r="F190" t="s">
+      <c r="F190" s="19" t="s">
         <v>337</v>
       </c>
       <c r="G190" t="s">
@@ -10386,7 +10394,7 @@
       <c r="D191">
         <v>2</v>
       </c>
-      <c r="F191" t="s">
+      <c r="F191" s="19" t="s">
         <v>338</v>
       </c>
       <c r="G191" t="s">
@@ -10412,7 +10420,7 @@
       <c r="D192">
         <v>2</v>
       </c>
-      <c r="F192" t="s">
+      <c r="F192" s="19" t="s">
         <v>556</v>
       </c>
       <c r="G192" t="s">
@@ -10438,7 +10446,7 @@
       <c r="D193">
         <v>2</v>
       </c>
-      <c r="F193" t="s">
+      <c r="F193" s="19" t="s">
         <v>340</v>
       </c>
       <c r="G193" t="s">
@@ -10464,7 +10472,7 @@
       <c r="D194">
         <v>2</v>
       </c>
-      <c r="F194" t="s">
+      <c r="F194" s="19" t="s">
         <v>341</v>
       </c>
       <c r="G194" t="s">
@@ -10490,7 +10498,7 @@
       <c r="D195">
         <v>0</v>
       </c>
-      <c r="E195">
+      <c r="E195" s="19">
         <v>4000</v>
       </c>
       <c r="G195" t="s">
@@ -10556,7 +10564,7 @@
       <c r="D198">
         <v>4</v>
       </c>
-      <c r="E198">
+      <c r="E198" s="19">
         <v>4000</v>
       </c>
       <c r="G198" s="14" t="s">
@@ -10611,7 +10619,7 @@
       <c r="D200">
         <v>2</v>
       </c>
-      <c r="F200" t="s">
+      <c r="F200" s="19" t="s">
         <v>344</v>
       </c>
       <c r="G200" t="s">
@@ -10637,7 +10645,7 @@
       <c r="D201">
         <v>2</v>
       </c>
-      <c r="E201">
+      <c r="E201" s="19">
         <v>4100</v>
       </c>
       <c r="G201" t="s">
@@ -10686,7 +10694,7 @@
       <c r="D203">
         <v>3</v>
       </c>
-      <c r="E203">
+      <c r="E203" s="19">
         <v>4110</v>
       </c>
       <c r="G203" t="s">
@@ -10712,7 +10720,7 @@
       <c r="D204">
         <v>2</v>
       </c>
-      <c r="E204">
+      <c r="E204" s="19">
         <v>4130</v>
       </c>
       <c r="G204" t="s">
@@ -10738,7 +10746,7 @@
       <c r="D205">
         <v>1</v>
       </c>
-      <c r="E205">
+      <c r="E205" s="19">
         <v>4140</v>
       </c>
       <c r="G205" t="s">
@@ -10764,7 +10772,7 @@
       <c r="D206">
         <v>2</v>
       </c>
-      <c r="F206" t="s">
+      <c r="F206" s="19" t="s">
         <v>557</v>
       </c>
       <c r="G206" t="s">
@@ -10790,7 +10798,7 @@
       <c r="D207">
         <v>2</v>
       </c>
-      <c r="F207" t="s">
+      <c r="F207" s="19" t="s">
         <v>351</v>
       </c>
       <c r="G207" t="s">
@@ -10816,7 +10824,7 @@
       <c r="D208">
         <v>2</v>
       </c>
-      <c r="E208">
+      <c r="E208" s="19">
         <v>4200</v>
       </c>
       <c r="G208" t="s">
@@ -10842,7 +10850,7 @@
       <c r="D209">
         <v>1</v>
       </c>
-      <c r="F209" t="s">
+      <c r="F209" s="19" t="s">
         <v>355</v>
       </c>
       <c r="G209" t="s">
@@ -10940,7 +10948,7 @@
       <c r="D213">
         <v>2</v>
       </c>
-      <c r="F213" t="s">
+      <c r="F213" s="19" t="s">
         <v>356</v>
       </c>
       <c r="G213" t="s">
@@ -10989,7 +10997,7 @@
       <c r="D215">
         <v>2</v>
       </c>
-      <c r="F215" t="s">
+      <c r="F215" s="19" t="s">
         <v>357</v>
       </c>
       <c r="G215" t="s">
@@ -11038,7 +11046,7 @@
       <c r="D217">
         <v>2</v>
       </c>
-      <c r="F217" t="s">
+      <c r="F217" s="19" t="s">
         <v>358</v>
       </c>
       <c r="G217" t="s">
@@ -11087,7 +11095,7 @@
       <c r="D219">
         <v>2</v>
       </c>
-      <c r="F219" t="s">
+      <c r="F219" s="19" t="s">
         <v>359</v>
       </c>
       <c r="G219" t="s">
@@ -11113,7 +11121,7 @@
       <c r="D220">
         <v>2</v>
       </c>
-      <c r="E220">
+      <c r="E220" s="19">
         <v>4230</v>
       </c>
       <c r="G220" t="s">
@@ -11139,7 +11147,7 @@
       <c r="D221">
         <v>1</v>
       </c>
-      <c r="E221">
+      <c r="E221" s="19">
         <v>4240</v>
       </c>
       <c r="G221" t="s">
@@ -11165,7 +11173,7 @@
       <c r="D222">
         <v>2</v>
       </c>
-      <c r="E222">
+      <c r="E222" s="19">
         <v>4250</v>
       </c>
       <c r="G222" t="s">
@@ -11214,7 +11222,7 @@
       <c r="D224">
         <v>2</v>
       </c>
-      <c r="E224">
+      <c r="E224" s="19">
         <v>6110</v>
       </c>
       <c r="G224" t="s">
@@ -11240,7 +11248,7 @@
       <c r="D225">
         <v>2</v>
       </c>
-      <c r="E225">
+      <c r="E225" s="19">
         <v>6400</v>
       </c>
       <c r="G225" t="s">
@@ -11286,7 +11294,7 @@
       <c r="D227">
         <v>3</v>
       </c>
-      <c r="E227">
+      <c r="E227" s="19">
         <v>6430</v>
       </c>
       <c r="G227" t="s">
@@ -11330,7 +11338,7 @@
       <c r="D229">
         <v>2</v>
       </c>
-      <c r="E229">
+      <c r="E229" s="19">
         <v>6440</v>
       </c>
       <c r="G229" t="s">
@@ -11379,7 +11387,7 @@
       <c r="D231">
         <v>3</v>
       </c>
-      <c r="E231">
+      <c r="E231" s="19">
         <v>6450</v>
       </c>
       <c r="G231" t="s">
@@ -11428,7 +11436,7 @@
       <c r="D233">
         <v>0</v>
       </c>
-      <c r="E233">
+      <c r="E233" s="19">
         <v>6480</v>
       </c>
       <c r="G233" t="s">
@@ -11500,7 +11508,7 @@
       <c r="D236">
         <v>3</v>
       </c>
-      <c r="E236">
+      <c r="E236" s="19">
         <v>6530</v>
       </c>
       <c r="G236" t="s">
@@ -11549,7 +11557,7 @@
       <c r="D238">
         <v>3</v>
       </c>
-      <c r="E238">
+      <c r="E238" s="19">
         <v>6540</v>
       </c>
       <c r="G238" t="s">
@@ -11590,7 +11598,7 @@
       <c r="D240">
         <v>5</v>
       </c>
-      <c r="E240">
+      <c r="E240" s="19">
         <v>6540</v>
       </c>
       <c r="K240"/>
@@ -11608,7 +11616,7 @@
       <c r="D241">
         <v>1</v>
       </c>
-      <c r="E241">
+      <c r="E241" s="19">
         <v>6550</v>
       </c>
       <c r="G241" t="s">
@@ -11634,7 +11642,7 @@
       <c r="D242">
         <v>1</v>
       </c>
-      <c r="F242" t="s">
+      <c r="F242" s="19" t="s">
         <v>375</v>
       </c>
       <c r="G242" t="s">
@@ -11660,7 +11668,7 @@
       <c r="D243">
         <v>3</v>
       </c>
-      <c r="E243">
+      <c r="E243" s="19">
         <v>7060</v>
       </c>
       <c r="G243" t="s">
@@ -11709,7 +11717,7 @@
       <c r="D245">
         <v>3</v>
       </c>
-      <c r="F245" t="s">
+      <c r="F245" s="19" t="s">
         <v>376</v>
       </c>
       <c r="G245" t="s">
@@ -11735,7 +11743,7 @@
       <c r="D246">
         <v>2</v>
       </c>
-      <c r="E246">
+      <c r="E246" s="19">
         <v>8020</v>
       </c>
       <c r="G246" t="s">
@@ -11761,7 +11769,7 @@
       <c r="D247">
         <v>1</v>
       </c>
-      <c r="F247" t="s">
+      <c r="F247" s="19" t="s">
         <v>379</v>
       </c>
       <c r="G247" t="s">
@@ -11787,7 +11795,7 @@
       <c r="D248">
         <v>2</v>
       </c>
-      <c r="E248">
+      <c r="E248" s="19">
         <v>8030</v>
       </c>
       <c r="G248" t="s">
@@ -11813,7 +11821,7 @@
       <c r="D249">
         <v>2</v>
       </c>
-      <c r="E249">
+      <c r="E249" s="19">
         <v>8040</v>
       </c>
       <c r="G249" t="s">
@@ -11839,7 +11847,7 @@
       <c r="D250">
         <v>2</v>
       </c>
-      <c r="E250">
+      <c r="E250" s="19">
         <v>8050</v>
       </c>
       <c r="G250" t="s">
@@ -11865,7 +11873,7 @@
       <c r="D251">
         <v>2</v>
       </c>
-      <c r="E251">
+      <c r="E251" s="19">
         <v>8060</v>
       </c>
       <c r="G251" t="s">
@@ -11914,7 +11922,7 @@
       <c r="D253">
         <v>3</v>
       </c>
-      <c r="E253">
+      <c r="E253" s="19">
         <v>8070</v>
       </c>
       <c r="G253" t="s">
@@ -11942,7 +11950,7 @@
       <c r="D254">
         <v>2</v>
       </c>
-      <c r="E254">
+      <c r="E254" s="19">
         <v>8080</v>
       </c>
       <c r="G254" t="s">
@@ -11968,7 +11976,7 @@
       <c r="D255">
         <v>2</v>
       </c>
-      <c r="E255">
+      <c r="E255" s="19">
         <v>8090</v>
       </c>
       <c r="G255" t="s">
@@ -11994,7 +12002,7 @@
       <c r="D256">
         <v>0</v>
       </c>
-      <c r="E256" t="s">
+      <c r="E256" s="19" t="s">
         <v>612</v>
       </c>
       <c r="K256"/>
@@ -12035,7 +12043,7 @@
       <c r="D258">
         <v>0</v>
       </c>
-      <c r="E258" t="s">
+      <c r="E258" s="19" t="s">
         <v>613</v>
       </c>
       <c r="K258"/>
@@ -24148,88 +24156,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Classificatie xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">Intern</Classificatie>
-    <Entiteit_x0020_type xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">Record</Entiteit_x0020_type>
-    <_dlc_DocId xmlns="fbe582d4-4cd9-4e01-adc0-428c7d30a990">PNHZET2ZRHHM-1647798991-93060</_dlc_DocId>
-    <Aggregatieniveau xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">Archiefstuk</Aggregatieniveau>
-    <TaxCatchAll xmlns="d59e9867-4acc-40d5-91da-91f4047d1695"/>
-    <Omschrijving xmlns="d59e9867-4acc-40d5-91da-91f4047d1695" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <Aanmaakdatum xmlns="d59e9867-4acc-40d5-91da-91f4047d1695" xsi:nil="true"/>
-    <Document_x0020_type xmlns="d59e9867-4acc-40d5-91da-91f4047d1695" xsi:nil="true"/>
-    <_dlc_DocIdUrl xmlns="fbe582d4-4cd9-4e01-adc0-428c7d30a990">
-      <Url>https://waternet.sharepoint.com/sites/0182/_layouts/15/DocIdRedir.aspx?ID=PNHZET2ZRHHM-1647798991-93060</Url>
-      <Description>PNHZET2ZRHHM-1647798991-93060</Description>
-    </_dlc_DocIdUrl>
-    <Identificatiekenmerk xmlns="d59e9867-4acc-40d5-91da-91f4047d1695" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Algemeen - Word" ma:contentTypeID="0x0101004F34529632943E4DBB820B36F0ABAA0606010086381A6D56669A4DB59F7772448721B1" ma:contentTypeVersion="5" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="8fe95572a7a7878b61abe4cdcaa95a61">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d59e9867-4acc-40d5-91da-91f4047d1695" xmlns:ns3="fbe582d4-4cd9-4e01-adc0-428c7d30a990" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b624776c1a3c75443e1a1b758f5efa1" ns2:_="" ns3:_="">
     <xsd:import namespace="d59e9867-4acc-40d5-91da-91f4047d1695"/>
@@ -24529,45 +24455,94 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Classificatie xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">Intern</Classificatie>
+    <Entiteit_x0020_type xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">Record</Entiteit_x0020_type>
+    <_dlc_DocId xmlns="fbe582d4-4cd9-4e01-adc0-428c7d30a990">PNHZET2ZRHHM-1647798991-93060</_dlc_DocId>
+    <Aggregatieniveau xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">Archiefstuk</Aggregatieniveau>
+    <TaxCatchAll xmlns="d59e9867-4acc-40d5-91da-91f4047d1695"/>
+    <Omschrijving xmlns="d59e9867-4acc-40d5-91da-91f4047d1695" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="d59e9867-4acc-40d5-91da-91f4047d1695">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Aanmaakdatum xmlns="d59e9867-4acc-40d5-91da-91f4047d1695" xsi:nil="true"/>
+    <Document_x0020_type xmlns="d59e9867-4acc-40d5-91da-91f4047d1695" xsi:nil="true"/>
+    <_dlc_DocIdUrl xmlns="fbe582d4-4cd9-4e01-adc0-428c7d30a990">
+      <Url>https://waternet.sharepoint.com/sites/0182/_layouts/15/DocIdRedir.aspx?ID=PNHZET2ZRHHM-1647798991-93060</Url>
+      <Description>PNHZET2ZRHHM-1647798991-93060</Description>
+    </_dlc_DocIdUrl>
+    <Identificatiekenmerk xmlns="d59e9867-4acc-40d5-91da-91f4047d1695" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="7c1d69d6-3248-424b-85a1-c0d9ad05b603" ContentTypeId="0x0101004F34529632943E4DBB820B36F0ABAA060601" PreviousValue="false"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C93CFFD-81C7-408F-9360-B07E2D660303}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D2BE5C7-D2B0-4B18-9D85-BE52E70FE1F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{629D2343-3DBC-4425-9979-C53AF3E8F60A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="fbe582d4-4cd9-4e01-adc0-428c7d30a990"/>
-    <ds:schemaRef ds:uri="d59e9867-4acc-40d5-91da-91f4047d1695"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{743CA991-A91A-4ABA-A663-E5C279512219}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24586,6 +24561,39 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{629D2343-3DBC-4425-9979-C53AF3E8F60A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="fbe582d4-4cd9-4e01-adc0-428c7d30a990"/>
+    <ds:schemaRef ds:uri="d59e9867-4acc-40d5-91da-91f4047d1695"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D2BE5C7-D2B0-4B18-9D85-BE52E70FE1F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C93CFFD-81C7-408F-9360-B07E2D660303}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A66FD23B-6941-41A1-8A1A-FC46E735FC7F}">
   <ds:schemaRefs>

</xml_diff>